<commit_message>
Scenario for live server
</commit_message>
<xml_diff>
--- a/ScenarioData.xlsx
+++ b/ScenarioData.xlsx
@@ -396,10 +396,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{"IP":"13.124.88.115", "PORT":8300}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1-4 플레이</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -429,6 +425,10 @@
   </si>
   <si>
     <t>1-3 플레이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"IP":"live.lhv.kakaogames.com", "PORT":8300}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -802,18 +802,30 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -823,12 +835,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -840,12 +846,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1134,8 +1134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M118"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.100000000000001" customHeight="1"/>
@@ -1155,17 +1155,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="55.15" customHeight="1">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="32"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="36"/>
     </row>
     <row r="2" spans="1:13" ht="17.45" customHeight="1">
       <c r="A2" s="21"/>
@@ -1178,11 +1178,11 @@
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
-      <c r="G2" s="35">
+      <c r="G2" s="37">
         <v>42817</v>
       </c>
-      <c r="H2" s="35"/>
-      <c r="I2" s="36"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="38"/>
     </row>
     <row r="3" spans="1:13" ht="19.5" customHeight="1">
       <c r="A3" s="4" t="s">
@@ -1215,10 +1215,10 @@
       <c r="K3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="26" t="s">
+      <c r="L3" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="27"/>
+      <c r="M3" s="33"/>
     </row>
     <row r="4" spans="1:13" s="5" customFormat="1" ht="18.75" customHeight="1">
       <c r="A4" s="14">
@@ -1240,7 +1240,7 @@
         <v>24</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="6"/>
@@ -1310,7 +1310,7 @@
       <c r="A7" s="16">
         <v>4</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="30" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="15" t="s">
@@ -1335,7 +1335,7 @@
       <c r="A8" s="16">
         <v>5</v>
       </c>
-      <c r="B8" s="34"/>
+      <c r="B8" s="31"/>
       <c r="C8" s="15" t="s">
         <v>21</v>
       </c>
@@ -1451,11 +1451,11 @@
       <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:13" s="5" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A13" s="39">
+      <c r="A13" s="26">
         <v>4</v>
       </c>
-      <c r="B13" s="33" t="s">
-        <v>89</v>
+      <c r="B13" s="30" t="s">
+        <v>88</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>20</v>
@@ -1470,16 +1470,16 @@
         <v>27</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H13" s="8"/>
       <c r="I13" s="6"/>
     </row>
     <row r="14" spans="1:13" s="5" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A14" s="39">
+      <c r="A14" s="26">
         <v>5</v>
       </c>
-      <c r="B14" s="34"/>
+      <c r="B14" s="31"/>
       <c r="C14" s="15" t="s">
         <v>21</v>
       </c>
@@ -1493,17 +1493,17 @@
         <v>28</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H14" s="8"/>
       <c r="I14" s="6"/>
     </row>
     <row r="15" spans="1:13" s="5" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A15" s="39">
+      <c r="A15" s="26">
         <v>6</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>20</v>
@@ -1518,13 +1518,13 @@
         <v>27</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H15" s="8"/>
       <c r="I15" s="6"/>
     </row>
     <row r="16" spans="1:13" s="5" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A16" s="39">
+      <c r="A16" s="26">
         <v>7</v>
       </c>
       <c r="B16" s="29"/>
@@ -1541,13 +1541,13 @@
         <v>28</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H16" s="8"/>
       <c r="I16" s="6"/>
     </row>
     <row r="17" spans="1:9" s="5" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A17" s="39">
+      <c r="A17" s="26">
         <v>8</v>
       </c>
       <c r="B17" s="16" t="s">
@@ -1572,10 +1572,10 @@
       <c r="I17" s="6"/>
     </row>
     <row r="18" spans="1:9" s="5" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A18" s="39">
+      <c r="A18" s="26">
         <v>9</v>
       </c>
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="27" t="s">
         <v>39</v>
       </c>
       <c r="C18" s="15" t="s">
@@ -1597,7 +1597,7 @@
       <c r="I18" s="6"/>
     </row>
     <row r="19" spans="1:9" s="5" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A19" s="39">
+      <c r="A19" s="26">
         <v>10</v>
       </c>
       <c r="B19" s="16" t="s">
@@ -1622,7 +1622,7 @@
       <c r="I19" s="6"/>
     </row>
     <row r="20" spans="1:9" s="5" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A20" s="39">
+      <c r="A20" s="26">
         <v>11</v>
       </c>
       <c r="B20" s="16" t="s">
@@ -1647,11 +1647,11 @@
       <c r="I20" s="6"/>
     </row>
     <row r="21" spans="1:9" s="5" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A21" s="39">
+      <c r="A21" s="26">
         <v>13</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C21" s="15" t="s">
         <v>20</v>
@@ -1672,7 +1672,7 @@
       <c r="I21" s="6"/>
     </row>
     <row r="22" spans="1:9" s="5" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A22" s="39">
+      <c r="A22" s="26">
         <v>14</v>
       </c>
       <c r="B22" s="29"/>
@@ -1695,10 +1695,10 @@
       <c r="I22" s="6"/>
     </row>
     <row r="23" spans="1:9" s="5" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A23" s="39">
+      <c r="A23" s="26">
         <v>15</v>
       </c>
-      <c r="B23" s="33" t="s">
+      <c r="B23" s="30" t="s">
         <v>22</v>
       </c>
       <c r="C23" s="15" t="s">
@@ -1720,10 +1720,10 @@
       <c r="I23" s="6"/>
     </row>
     <row r="24" spans="1:9" s="5" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A24" s="39">
+      <c r="A24" s="26">
         <v>16</v>
       </c>
-      <c r="B24" s="34"/>
+      <c r="B24" s="31"/>
       <c r="C24" s="15" t="s">
         <v>21</v>
       </c>
@@ -1743,11 +1743,11 @@
       <c r="I24" s="6"/>
     </row>
     <row r="25" spans="1:9" s="5" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A25" s="39">
+      <c r="A25" s="26">
         <v>17</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C25" s="15" t="s">
         <v>20</v>
@@ -1768,7 +1768,7 @@
       <c r="I25" s="6"/>
     </row>
     <row r="26" spans="1:9" s="5" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A26" s="39">
+      <c r="A26" s="26">
         <v>18</v>
       </c>
       <c r="B26" s="29"/>
@@ -1791,11 +1791,11 @@
       <c r="I26" s="6"/>
     </row>
     <row r="27" spans="1:9" s="5" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A27" s="39">
+      <c r="A27" s="26">
         <v>19</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C27" s="15" t="s">
         <v>20</v>
@@ -1810,13 +1810,13 @@
         <v>27</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H27" s="8"/>
       <c r="I27" s="6"/>
     </row>
     <row r="28" spans="1:9" s="5" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A28" s="39">
+      <c r="A28" s="26">
         <v>20</v>
       </c>
       <c r="B28" s="29"/>
@@ -1833,17 +1833,17 @@
         <v>28</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H28" s="8"/>
       <c r="I28" s="6"/>
     </row>
     <row r="29" spans="1:9" s="5" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A29" s="39">
+      <c r="A29" s="26">
         <v>21</v>
       </c>
-      <c r="B29" s="33" t="s">
-        <v>92</v>
+      <c r="B29" s="30" t="s">
+        <v>91</v>
       </c>
       <c r="C29" s="15" t="s">
         <v>20</v>
@@ -1858,16 +1858,16 @@
         <v>27</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H29" s="8"/>
       <c r="I29" s="6"/>
     </row>
     <row r="30" spans="1:9" s="5" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A30" s="39">
+      <c r="A30" s="26">
         <v>22</v>
       </c>
-      <c r="B30" s="34"/>
+      <c r="B30" s="31"/>
       <c r="C30" s="15" t="s">
         <v>21</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>28</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H30" s="8"/>
       <c r="I30" s="6"/>
@@ -2871,6 +2871,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="G2:I2"/>
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="B29:B30"/>
     <mergeCell ref="B13:B14"/>
@@ -2878,13 +2885,6 @@
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="B25:B26"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="G2:I2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3000,7 +3000,7 @@
       <c r="D10" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="37" t="s">
+      <c r="E10" s="39" t="s">
         <v>66</v>
       </c>
       <c r="F10" s="6" t="s">
@@ -3020,7 +3020,7 @@
       <c r="D11" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E11" s="38"/>
+      <c r="E11" s="40"/>
       <c r="F11" s="6" t="s">
         <v>73</v>
       </c>

</xml_diff>